<commit_message>
reduced ARC orifice coefficients
</commit_message>
<xml_diff>
--- a/oxide/ARC/physicalImplementation/variables.xlsx
+++ b/oxide/ARC/physicalImplementation/variables.xlsx
@@ -675,7 +675,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -767,10 +767,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,7 +1277,7 @@
         <v>142</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5" t="s">
         <v>160</v>
@@ -1321,7 +1321,7 @@
         <v>141</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D6" t="s">
         <v>160</v>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="I77" s="7">
         <f>B5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J77" t="s">
         <v>139</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="I78" s="7">
         <f>B6</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J78" t="s">
         <v>140</v>
@@ -4551,7 +4551,7 @@
       </c>
       <c r="I82" s="7">
         <f>B6</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J82" t="s">
         <v>138</v>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="I83" s="7">
         <f>B5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J83" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
made fixes to the flow area and hydraulic diameter which were due to an error in the FTF distance
</commit_message>
<xml_diff>
--- a/oxide/ARC/physicalImplementation/variables.xlsx
+++ b/oxide/ARC/physicalImplementation/variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51120" yWindow="440" windowWidth="51120" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="-51120" yWindow="440" windowWidth="25560" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,7 +1471,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="1">
-        <v>14.92</v>
+        <v>0.1492</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1542,10 +1542,10 @@
         <v>40</v>
       </c>
       <c r="H10" s="1">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="I10" s="6">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="L10" t="s">
         <v>40</v>
@@ -1586,10 +1586,10 @@
         <v>41</v>
       </c>
       <c r="H11" s="1">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="I11" s="6">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="L11" t="s">
         <v>41</v>
@@ -1636,7 +1636,8 @@
         <v>36</v>
       </c>
       <c r="I12" s="6">
-        <v>2.5398999999999999E-5</v>
+        <f>(3/2/SQRT(3)*B9^2 - PI()*B10^2)/B11</f>
+        <v>7.0971924029625367E-5</v>
       </c>
       <c r="J12" t="s">
         <v>49</v>
@@ -1689,7 +1690,8 @@
         <v>36</v>
       </c>
       <c r="I13" s="6">
-        <v>2.5398999999999999E-5</v>
+        <f>(3/2/SQRT(3)*B9^2 - PI()*(B8^2-B7^2))/B11</f>
+        <v>5.5636064442975235E-5</v>
       </c>
       <c r="J13" t="s">
         <v>43</v>
@@ -1739,10 +1741,10 @@
         <v>44</v>
       </c>
       <c r="H14" s="1">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="I14" s="6">
-        <v>2.5398999999999999E-5</v>
+        <v>2.5026599999999999E-5</v>
       </c>
       <c r="J14" t="s">
         <v>62</v>
@@ -1872,7 +1874,7 @@
       </c>
       <c r="I17" s="6">
         <f>4*I12*B11/(B9/2/SQRT(3)*12+PI()*2*B10)</f>
-        <v>5.3245992833253139E-4</v>
+        <v>0.14231291601101889</v>
       </c>
       <c r="J17" t="s">
         <v>55</v>
@@ -1920,7 +1922,7 @@
       </c>
       <c r="I18" s="6">
         <f>4*I13*B11/(B9/2/SQRT(3)*12+2*PI()*B7+2*PI()*B8)</f>
-        <v>5.2731341130203687E-4</v>
+        <v>5.7698087347996037E-2</v>
       </c>
       <c r="J18" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
made correct ULOHS deck with physical implementation of ARC reservoir. discovered that I was missing edits to XKSTIZ and XKSTOZ
</commit_message>
<xml_diff>
--- a/oxide/ARC/physicalImplementation/variables.xlsx
+++ b/oxide/ARC/physicalImplementation/variables.xlsx
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="174">
   <si>
     <t>Lower Reservoir Height</t>
   </si>
@@ -668,6 +668,36 @@
   </si>
   <si>
     <t>ULOF</t>
+  </si>
+  <si>
+    <t>XKSTIZ(1)</t>
+  </si>
+  <si>
+    <t>XKSTIZ(2)</t>
+  </si>
+  <si>
+    <t>XKSTIZ(3)</t>
+  </si>
+  <si>
+    <t>XKSTIZ(4)</t>
+  </si>
+  <si>
+    <t>XKSTIZ(5)</t>
+  </si>
+  <si>
+    <t>XKSTOZ(1)</t>
+  </si>
+  <si>
+    <t>XKSTOZ(2)</t>
+  </si>
+  <si>
+    <t>XKSTOZ(3)</t>
+  </si>
+  <si>
+    <t>XKSTOZ(4)</t>
+  </si>
+  <si>
+    <t>XKSTOZ(5)</t>
   </si>
 </sst>
 </file>
@@ -751,7 +781,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -759,8 +789,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -774,17 +806,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1088,11 +1143,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T93"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5049,19 +5102,411 @@
         <v>36</v>
       </c>
     </row>
+    <row r="94" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>160</v>
+      </c>
+      <c r="E94" t="s">
+        <v>159</v>
+      </c>
+      <c r="F94" t="s">
+        <v>159</v>
+      </c>
+      <c r="G94" t="s">
+        <v>164</v>
+      </c>
+      <c r="H94" s="1">
+        <v>26</v>
+      </c>
+      <c r="I94" s="13">
+        <v>26</v>
+      </c>
+      <c r="L94" t="s">
+        <v>164</v>
+      </c>
+      <c r="M94" t="s">
+        <v>36</v>
+      </c>
+      <c r="N94" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>164</v>
+      </c>
+      <c r="R94" t="s">
+        <v>36</v>
+      </c>
+      <c r="S94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>160</v>
+      </c>
+      <c r="E95" t="s">
+        <v>159</v>
+      </c>
+      <c r="F95" t="s">
+        <v>159</v>
+      </c>
+      <c r="G95" t="s">
+        <v>165</v>
+      </c>
+      <c r="H95" s="1">
+        <v>26</v>
+      </c>
+      <c r="I95" s="13">
+        <v>26</v>
+      </c>
+      <c r="L95" t="s">
+        <v>165</v>
+      </c>
+      <c r="M95" t="s">
+        <v>36</v>
+      </c>
+      <c r="N95" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>165</v>
+      </c>
+      <c r="R95" t="s">
+        <v>36</v>
+      </c>
+      <c r="S95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>160</v>
+      </c>
+      <c r="E96" t="s">
+        <v>159</v>
+      </c>
+      <c r="F96" t="s">
+        <v>159</v>
+      </c>
+      <c r="G96" t="s">
+        <v>166</v>
+      </c>
+      <c r="H96" t="s">
+        <v>36</v>
+      </c>
+      <c r="I96" s="13">
+        <v>26</v>
+      </c>
+      <c r="J96" t="s">
+        <v>65</v>
+      </c>
+      <c r="L96" t="s">
+        <v>166</v>
+      </c>
+      <c r="M96" t="s">
+        <v>36</v>
+      </c>
+      <c r="N96" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>166</v>
+      </c>
+      <c r="R96" t="s">
+        <v>36</v>
+      </c>
+      <c r="S96" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>160</v>
+      </c>
+      <c r="E97" t="s">
+        <v>159</v>
+      </c>
+      <c r="F97" t="s">
+        <v>159</v>
+      </c>
+      <c r="G97" t="s">
+        <v>167</v>
+      </c>
+      <c r="H97" t="s">
+        <v>36</v>
+      </c>
+      <c r="I97" s="13">
+        <v>26</v>
+      </c>
+      <c r="J97" t="s">
+        <v>65</v>
+      </c>
+      <c r="L97" t="s">
+        <v>167</v>
+      </c>
+      <c r="M97" t="s">
+        <v>36</v>
+      </c>
+      <c r="N97" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>167</v>
+      </c>
+      <c r="R97" t="s">
+        <v>36</v>
+      </c>
+      <c r="S97" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>160</v>
+      </c>
+      <c r="E98" t="s">
+        <v>159</v>
+      </c>
+      <c r="F98" t="s">
+        <v>159</v>
+      </c>
+      <c r="G98" t="s">
+        <v>168</v>
+      </c>
+      <c r="H98" s="1">
+        <v>26</v>
+      </c>
+      <c r="I98" s="13">
+        <v>26</v>
+      </c>
+      <c r="L98" t="s">
+        <v>168</v>
+      </c>
+      <c r="M98" t="s">
+        <v>36</v>
+      </c>
+      <c r="N98" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>168</v>
+      </c>
+      <c r="R98" t="s">
+        <v>36</v>
+      </c>
+      <c r="S98" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>160</v>
+      </c>
+      <c r="E99" t="s">
+        <v>159</v>
+      </c>
+      <c r="F99" t="s">
+        <v>159</v>
+      </c>
+      <c r="G99" t="s">
+        <v>169</v>
+      </c>
+      <c r="H99" s="1">
+        <v>26</v>
+      </c>
+      <c r="I99" s="13">
+        <v>26</v>
+      </c>
+      <c r="L99" t="s">
+        <v>169</v>
+      </c>
+      <c r="M99" t="s">
+        <v>36</v>
+      </c>
+      <c r="N99" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>169</v>
+      </c>
+      <c r="R99" t="s">
+        <v>36</v>
+      </c>
+      <c r="S99" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>160</v>
+      </c>
+      <c r="E100" t="s">
+        <v>159</v>
+      </c>
+      <c r="F100" t="s">
+        <v>159</v>
+      </c>
+      <c r="G100" t="s">
+        <v>170</v>
+      </c>
+      <c r="H100" s="1">
+        <v>26</v>
+      </c>
+      <c r="I100" s="13">
+        <v>26</v>
+      </c>
+      <c r="L100" t="s">
+        <v>170</v>
+      </c>
+      <c r="M100" t="s">
+        <v>36</v>
+      </c>
+      <c r="N100" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>170</v>
+      </c>
+      <c r="R100" t="s">
+        <v>36</v>
+      </c>
+      <c r="S100" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>160</v>
+      </c>
+      <c r="E101" t="s">
+        <v>159</v>
+      </c>
+      <c r="F101" t="s">
+        <v>159</v>
+      </c>
+      <c r="G101" t="s">
+        <v>171</v>
+      </c>
+      <c r="H101" t="s">
+        <v>36</v>
+      </c>
+      <c r="I101" s="13">
+        <v>26</v>
+      </c>
+      <c r="J101" t="s">
+        <v>65</v>
+      </c>
+      <c r="L101" t="s">
+        <v>171</v>
+      </c>
+      <c r="M101" t="s">
+        <v>36</v>
+      </c>
+      <c r="N101" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>171</v>
+      </c>
+      <c r="R101" t="s">
+        <v>36</v>
+      </c>
+      <c r="S101" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>160</v>
+      </c>
+      <c r="E102" t="s">
+        <v>159</v>
+      </c>
+      <c r="F102" t="s">
+        <v>159</v>
+      </c>
+      <c r="G102" t="s">
+        <v>172</v>
+      </c>
+      <c r="H102" t="s">
+        <v>36</v>
+      </c>
+      <c r="I102" s="13">
+        <v>26</v>
+      </c>
+      <c r="J102" t="s">
+        <v>65</v>
+      </c>
+      <c r="L102" t="s">
+        <v>172</v>
+      </c>
+      <c r="M102" t="s">
+        <v>36</v>
+      </c>
+      <c r="N102" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>172</v>
+      </c>
+      <c r="R102" t="s">
+        <v>36</v>
+      </c>
+      <c r="S102" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="103" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>160</v>
+      </c>
+      <c r="E103" t="s">
+        <v>159</v>
+      </c>
+      <c r="F103" t="s">
+        <v>159</v>
+      </c>
+      <c r="G103" t="s">
+        <v>173</v>
+      </c>
+      <c r="H103" s="1">
+        <v>26</v>
+      </c>
+      <c r="I103" s="13">
+        <v>26</v>
+      </c>
+      <c r="L103" t="s">
+        <v>173</v>
+      </c>
+      <c r="M103" t="s">
+        <v>36</v>
+      </c>
+      <c r="N103" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>173</v>
+      </c>
+      <c r="R103" t="s">
+        <v>36</v>
+      </c>
+      <c r="S103" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D93">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N">
+  <conditionalFormatting sqref="D3:D103">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E93">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N">
+  <conditionalFormatting sqref="E3:E103">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F93">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N">
+  <conditionalFormatting sqref="F3:F103">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",F3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed error in UTOP
</commit_message>
<xml_diff>
--- a/oxide/ARC/physicalImplementation/variables.xlsx
+++ b/oxide/ARC/physicalImplementation/variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51120" yWindow="440" windowWidth="25560" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,17 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1145,7 +1155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1241,7 +1253,7 @@
         <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
         <v>159</v>
@@ -1292,7 +1304,7 @@
         <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
         <v>159</v>
@@ -1336,7 +1348,7 @@
         <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
         <v>159</v>
@@ -1380,7 +1392,7 @@
         <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
         <v>159</v>
@@ -1427,7 +1439,7 @@
         <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>159</v>
@@ -1480,7 +1492,7 @@
         <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F8" t="s">
         <v>159</v>
@@ -1533,7 +1545,7 @@
         <v>160</v>
       </c>
       <c r="E9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
         <v>159</v>
@@ -1586,7 +1598,7 @@
         <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F10" t="s">
         <v>159</v>
@@ -1630,7 +1642,7 @@
         <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
         <v>159</v>
@@ -1677,7 +1689,7 @@
         <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F12" t="s">
         <v>159</v>
@@ -1731,7 +1743,7 @@
         <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F13" t="s">
         <v>159</v>
@@ -1785,7 +1797,7 @@
         <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F14" t="s">
         <v>159</v>
@@ -1838,7 +1850,7 @@
         <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F15" t="s">
         <v>159</v>
@@ -1876,7 +1888,7 @@
         <v>160</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F16" t="s">
         <v>159</v>
@@ -1914,7 +1926,7 @@
         <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
         <v>159</v>
@@ -1962,7 +1974,7 @@
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
         <v>159</v>
@@ -2014,7 +2026,7 @@
         <v>160</v>
       </c>
       <c r="E19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
         <v>159</v>
@@ -2067,7 +2079,7 @@
         <v>160</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F20" t="s">
         <v>159</v>
@@ -2114,7 +2126,7 @@
         <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F21" t="s">
         <v>159</v>
@@ -2161,7 +2173,7 @@
         <v>160</v>
       </c>
       <c r="E22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
         <v>159</v>
@@ -2205,7 +2217,7 @@
         <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F23" t="s">
         <v>159</v>
@@ -2249,7 +2261,7 @@
         <v>160</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
         <v>159</v>
@@ -2290,7 +2302,7 @@
         <v>160</v>
       </c>
       <c r="E25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F25" t="s">
         <v>159</v>
@@ -2334,7 +2346,7 @@
         <v>160</v>
       </c>
       <c r="E26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F26" t="s">
         <v>159</v>
@@ -2372,7 +2384,7 @@
         <v>160</v>
       </c>
       <c r="E27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F27" t="s">
         <v>159</v>
@@ -2416,7 +2428,7 @@
         <v>160</v>
       </c>
       <c r="E28" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F28" t="s">
         <v>159</v>
@@ -2460,7 +2472,7 @@
         <v>160</v>
       </c>
       <c r="E29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F29" t="s">
         <v>159</v>
@@ -2498,7 +2510,7 @@
         <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F30" t="s">
         <v>159</v>
@@ -2536,7 +2548,7 @@
         <v>160</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F31" t="s">
         <v>159</v>
@@ -2574,7 +2586,7 @@
         <v>160</v>
       </c>
       <c r="E32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F32" t="s">
         <v>159</v>
@@ -2618,7 +2630,7 @@
         <v>160</v>
       </c>
       <c r="E33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F33" t="s">
         <v>159</v>
@@ -2663,7 +2675,7 @@
         <v>160</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F34" t="s">
         <v>159</v>
@@ -2701,7 +2713,7 @@
         <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
         <v>159</v>
@@ -2739,7 +2751,7 @@
         <v>160</v>
       </c>
       <c r="E36" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F36" t="s">
         <v>159</v>
@@ -2777,7 +2789,7 @@
         <v>160</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F37" t="s">
         <v>159</v>
@@ -2821,7 +2833,7 @@
         <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F38" t="s">
         <v>159</v>
@@ -2866,7 +2878,7 @@
         <v>160</v>
       </c>
       <c r="E39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F39" t="s">
         <v>159</v>
@@ -2904,7 +2916,7 @@
         <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F40" t="s">
         <v>159</v>
@@ -2942,7 +2954,7 @@
         <v>160</v>
       </c>
       <c r="E41" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F41" t="s">
         <v>159</v>
@@ -2980,7 +2992,7 @@
         <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F42" t="s">
         <v>159</v>
@@ -3025,7 +3037,7 @@
         <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F43" t="s">
         <v>159</v>
@@ -3070,7 +3082,7 @@
         <v>160</v>
       </c>
       <c r="E44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F44" t="s">
         <v>159</v>
@@ -3108,7 +3120,7 @@
         <v>160</v>
       </c>
       <c r="E45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F45" t="s">
         <v>159</v>
@@ -3146,7 +3158,7 @@
         <v>160</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F46" t="s">
         <v>159</v>
@@ -3184,7 +3196,7 @@
         <v>160</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F47" t="s">
         <v>159</v>
@@ -3230,7 +3242,7 @@
         <v>160</v>
       </c>
       <c r="E48" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F48" t="s">
         <v>159</v>
@@ -3276,7 +3288,7 @@
         <v>160</v>
       </c>
       <c r="E49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F49" t="s">
         <v>159</v>
@@ -3320,7 +3332,7 @@
         <v>160</v>
       </c>
       <c r="E50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F50" t="s">
         <v>159</v>
@@ -3358,7 +3370,7 @@
         <v>160</v>
       </c>
       <c r="E51" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F51" t="s">
         <v>159</v>
@@ -3396,7 +3408,7 @@
         <v>160</v>
       </c>
       <c r="E52" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F52" t="s">
         <v>159</v>
@@ -3440,7 +3452,7 @@
         <v>160</v>
       </c>
       <c r="E53" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F53" t="s">
         <v>159</v>
@@ -3484,7 +3496,7 @@
         <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F54" t="s">
         <v>159</v>
@@ -3522,7 +3534,7 @@
         <v>160</v>
       </c>
       <c r="E55" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F55" t="s">
         <v>159</v>
@@ -3560,7 +3572,7 @@
         <v>160</v>
       </c>
       <c r="E56" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F56" t="s">
         <v>159</v>
@@ -3598,7 +3610,7 @@
         <v>160</v>
       </c>
       <c r="E57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F57" t="s">
         <v>159</v>
@@ -3639,7 +3651,7 @@
         <v>160</v>
       </c>
       <c r="E58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F58" t="s">
         <v>159</v>
@@ -3680,7 +3692,7 @@
         <v>160</v>
       </c>
       <c r="E59" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F59" t="s">
         <v>159</v>
@@ -3718,7 +3730,7 @@
         <v>160</v>
       </c>
       <c r="E60" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F60" t="s">
         <v>159</v>
@@ -3756,7 +3768,7 @@
         <v>160</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F61" t="s">
         <v>159</v>
@@ -3794,7 +3806,7 @@
         <v>160</v>
       </c>
       <c r="E62" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F62" t="s">
         <v>159</v>
@@ -3835,7 +3847,7 @@
         <v>160</v>
       </c>
       <c r="E63" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F63" t="s">
         <v>159</v>
@@ -3876,7 +3888,7 @@
         <v>160</v>
       </c>
       <c r="E64" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F64" t="s">
         <v>159</v>
@@ -3914,7 +3926,7 @@
         <v>160</v>
       </c>
       <c r="E65" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F65" t="s">
         <v>159</v>
@@ -3952,7 +3964,7 @@
         <v>160</v>
       </c>
       <c r="E66" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F66" t="s">
         <v>159</v>
@@ -3990,7 +4002,7 @@
         <v>160</v>
       </c>
       <c r="E67" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F67" t="s">
         <v>159</v>
@@ -4031,7 +4043,7 @@
         <v>160</v>
       </c>
       <c r="E68" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F68" t="s">
         <v>159</v>
@@ -4072,7 +4084,7 @@
         <v>160</v>
       </c>
       <c r="E69" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F69" t="s">
         <v>159</v>
@@ -4110,7 +4122,7 @@
         <v>160</v>
       </c>
       <c r="E70" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F70" t="s">
         <v>159</v>
@@ -4148,7 +4160,7 @@
         <v>160</v>
       </c>
       <c r="E71" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F71" t="s">
         <v>159</v>
@@ -4186,7 +4198,7 @@
         <v>160</v>
       </c>
       <c r="E72" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F72" t="s">
         <v>159</v>
@@ -4227,7 +4239,7 @@
         <v>160</v>
       </c>
       <c r="E73" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F73" t="s">
         <v>159</v>
@@ -4266,7 +4278,7 @@
         <v>160</v>
       </c>
       <c r="E74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F74" t="s">
         <v>159</v>
@@ -4307,7 +4319,7 @@
         <v>160</v>
       </c>
       <c r="E75" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F75" t="s">
         <v>159</v>
@@ -4345,7 +4357,7 @@
         <v>160</v>
       </c>
       <c r="E76" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F76" t="s">
         <v>159</v>
@@ -4389,7 +4401,7 @@
         <v>160</v>
       </c>
       <c r="E77" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F77" t="s">
         <v>159</v>
@@ -4434,7 +4446,7 @@
         <v>160</v>
       </c>
       <c r="E78" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F78" t="s">
         <v>159</v>
@@ -4479,7 +4491,7 @@
         <v>160</v>
       </c>
       <c r="E79" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F79" t="s">
         <v>159</v>
@@ -4517,7 +4529,7 @@
         <v>160</v>
       </c>
       <c r="E80" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F80" t="s">
         <v>159</v>
@@ -4555,7 +4567,7 @@
         <v>160</v>
       </c>
       <c r="E81" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F81" t="s">
         <v>159</v>
@@ -4593,7 +4605,7 @@
         <v>160</v>
       </c>
       <c r="E82" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F82" t="s">
         <v>159</v>
@@ -4638,7 +4650,7 @@
         <v>160</v>
       </c>
       <c r="E83" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F83" t="s">
         <v>159</v>
@@ -4683,7 +4695,7 @@
         <v>160</v>
       </c>
       <c r="E84" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F84" t="s">
         <v>159</v>
@@ -4721,7 +4733,7 @@
         <v>160</v>
       </c>
       <c r="E85" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F85" t="s">
         <v>159</v>
@@ -4760,7 +4772,7 @@
         <v>160</v>
       </c>
       <c r="E86" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F86" t="s">
         <v>159</v>
@@ -4799,7 +4811,7 @@
         <v>160</v>
       </c>
       <c r="E87" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F87" t="s">
         <v>159</v>
@@ -4843,7 +4855,7 @@
         <v>160</v>
       </c>
       <c r="E88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F88" t="s">
         <v>159</v>
@@ -4887,7 +4899,7 @@
         <v>160</v>
       </c>
       <c r="E89" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F89" t="s">
         <v>159</v>
@@ -4931,7 +4943,7 @@
         <v>160</v>
       </c>
       <c r="E90" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F90" t="s">
         <v>159</v>
@@ -4975,7 +4987,7 @@
         <v>160</v>
       </c>
       <c r="E91" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F91" t="s">
         <v>159</v>
@@ -5019,7 +5031,7 @@
         <v>160</v>
       </c>
       <c r="E92" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F92" t="s">
         <v>159</v>
@@ -5063,7 +5075,7 @@
         <v>160</v>
       </c>
       <c r="E93" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F93" t="s">
         <v>159</v>
@@ -5107,7 +5119,7 @@
         <v>160</v>
       </c>
       <c r="E94" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F94" t="s">
         <v>159</v>
@@ -5145,7 +5157,7 @@
         <v>160</v>
       </c>
       <c r="E95" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F95" t="s">
         <v>159</v>
@@ -5183,7 +5195,7 @@
         <v>160</v>
       </c>
       <c r="E96" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F96" t="s">
         <v>159</v>
@@ -5224,7 +5236,7 @@
         <v>160</v>
       </c>
       <c r="E97" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F97" t="s">
         <v>159</v>
@@ -5265,7 +5277,7 @@
         <v>160</v>
       </c>
       <c r="E98" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F98" t="s">
         <v>159</v>
@@ -5303,7 +5315,7 @@
         <v>160</v>
       </c>
       <c r="E99" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F99" t="s">
         <v>159</v>
@@ -5341,7 +5353,7 @@
         <v>160</v>
       </c>
       <c r="E100" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F100" t="s">
         <v>159</v>
@@ -5379,7 +5391,7 @@
         <v>160</v>
       </c>
       <c r="E101" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F101" t="s">
         <v>159</v>
@@ -5420,7 +5432,7 @@
         <v>160</v>
       </c>
       <c r="E102" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F102" t="s">
         <v>159</v>
@@ -5461,7 +5473,7 @@
         <v>160</v>
       </c>
       <c r="E103" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F103" t="s">
         <v>159</v>
@@ -5496,17 +5508,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D103">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E103">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F103">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",F3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>